<commit_message>
Fixed bug converting ts to C#
Error was given if ts value didn't have default value.
</commit_message>
<xml_diff>
--- a/convert c# to typescript - lower case.xlsx
+++ b/convert c# to typescript - lower case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://audacia-my.sharepoint.com/personal/tim_hilton_audacia_co_uk/Documents/Tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{14342027-79ED-4EE2-88B8-121A4C891E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE2C27D8-ED40-44C8-8DDE-C2424F98DD04}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{14342027-79ED-4EE2-88B8-121A4C891E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90ABB3B0-0DAB-46E8-A644-AD66384B3255}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C# model to ts" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
   <si>
     <t>Name</t>
   </si>
@@ -3865,8 +3865,11 @@
     <t>C# nullable type</t>
   </si>
   <si>
-    <r>
-      <t>Username</t>
+    <t>Type onwards</t>
+  </si>
+  <si>
+    <r>
+      <t>salesContractId</t>
     </r>
     <r>
       <rPr>
@@ -3884,16 +3887,30 @@
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">string </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
+      <t>number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>salesContractNumber</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
     </r>
     <r>
       <rPr>
@@ -3902,7 +3919,7 @@
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
       </rPr>
-      <t>null</t>
+      <t>string</t>
     </r>
     <r>
       <rPr>
@@ -3916,7 +3933,7 @@
   </si>
   <si>
     <r>
-      <t>Password</t>
+      <t>deliveryOrderNumber</t>
     </r>
     <r>
       <rPr>
@@ -3934,16 +3951,62 @@
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">string </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>tradingPeriod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFC191FF"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>currentPrice</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
     </r>
     <r>
       <rPr>
@@ -3952,7 +4015,7 @@
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
       </rPr>
-      <t>null</t>
+      <t>number</t>
     </r>
     <r>
       <rPr>
@@ -3966,7 +4029,7 @@
   </si>
   <si>
     <r>
-      <t>Host</t>
+      <t>proposedPrice</t>
     </r>
     <r>
       <rPr>
@@ -3984,16 +4047,30 @@
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">string </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
+      <t>number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>createdBy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
     </r>
     <r>
       <rPr>
@@ -4002,7 +4079,7 @@
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
       </rPr>
-      <t>null</t>
+      <t>string</t>
     </r>
     <r>
       <rPr>
@@ -4016,7 +4093,7 @@
   </si>
   <si>
     <r>
-      <t>Port</t>
+      <t>created</t>
     </r>
     <r>
       <rPr>
@@ -4030,29 +4107,43 @@
     <r>
       <rPr>
         <sz val="9.8000000000000007"/>
+        <color rgb="FFC191FF"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>currency</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFBDBDBD"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
         <color rgb="FF6C95EB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve">number </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>null</t>
+      <t>string</t>
     </r>
     <r>
       <rPr>
@@ -4065,214 +4156,35 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>EnableSsl</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">boolean </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>null</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>From</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">string </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>null</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>FromDisplayName</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">string </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>null</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>UseCredentials</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">boolean </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6C95EB"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>null</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFBDBDBD"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>;</t>
-    </r>
-  </si>
-  <si>
-    <t>Type onwards</t>
+    <t>Username: string = null;</t>
+  </si>
+  <si>
+    <t>Password: string = null;</t>
+  </si>
+  <si>
+    <t>Host: string = null;</t>
+  </si>
+  <si>
+    <t>Port: number = null;</t>
+  </si>
+  <si>
+    <t>EnableSsl: boolean = null;</t>
+  </si>
+  <si>
+    <t>From: string = null;</t>
+  </si>
+  <si>
+    <t>FromDisplayName: string = null;</t>
+  </si>
+  <si>
+    <t>UseCredentials: boolean = null;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4355,6 +4267,12 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FFE1BFFF"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFC191FF"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -9950,7 +9868,7 @@
   <dimension ref="A1:N90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9988,7 +9906,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>107</v>
@@ -10014,7 +9932,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B2">
         <f>LEN(A2)</f>
@@ -10022,15 +9940,15 @@
       </c>
       <c r="C2">
         <f>FIND(":", A2)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D2" t="str">
         <f>LEFT(A2,C2-1)</f>
-        <v>Username</v>
+        <v>salesContractId</v>
       </c>
       <c r="E2" t="str">
         <f>SUBSTITUTE(UPPER(LEFT(D2,1))&amp;RIGHT(D2, LEN(D2)-1),"?","")</f>
-        <v>Username</v>
+        <v>SalesContractId</v>
       </c>
       <c r="F2" t="b">
         <f>ISNUMBER(SEARCH("~?",D2))</f>
@@ -10038,11 +9956,11 @@
       </c>
       <c r="G2" t="str">
         <f>SUBSTITUTE(RIGHT(A2,B2-C2-1),";","")</f>
-        <v>string = null</v>
+        <v>number</v>
       </c>
       <c r="H2" t="str">
-        <f>IF(FIND("=",G2) &gt; -1, TRIM(LEFT(G2, FIND("=", G2) - 1)), G2)</f>
-        <v>string</v>
+        <f>IF(ISNUMBER(SEARCH("=",G2)), TRIM(LEFT(G2, FIND("=", G2) - 1)), G2)</f>
+        <v>number</v>
       </c>
       <c r="I2" t="b">
         <f>ISNUMBER(SEARCH("[]",G2))</f>
@@ -10050,44 +9968,44 @@
       </c>
       <c r="J2" t="str">
         <f>IF(I2,LEFT(H2,LEN(H2)-2),H2)</f>
-        <v>string</v>
+        <v>number</v>
       </c>
       <c r="K2" t="str">
         <f>IFERROR(VLOOKUP(J2,Types!$F$3:$G$7,2,FALSE),J2)</f>
-        <v>string</v>
+        <v>int</v>
       </c>
       <c r="L2" t="str">
         <f>IF(F2,K2&amp;"?",K2)</f>
-        <v>string</v>
+        <v>int</v>
       </c>
       <c r="M2" t="str">
         <f>IF(I2,"List&lt;"&amp;L2&amp;"&gt;",L2)</f>
-        <v>string</v>
+        <v>int</v>
       </c>
       <c r="N2" s="2" t="str">
         <f>"public "&amp;M2&amp;" "&amp;E2&amp;" { get; set; }"</f>
-        <v>public string Username { get; set; }</v>
+        <v>public int SalesContractId { get; set; }</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B4" si="0">LEN(A3)</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C4" si="1">FIND(":", A3)</f>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D4" si="2">LEFT(A3,C3-1)</f>
-        <v>Password</v>
+        <v>salesContractNumber</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E66" si="3">SUBSTITUTE(UPPER(LEFT(D3,1))&amp;RIGHT(D3, LEN(D3)-1),"?","")</f>
-        <v>Password</v>
+        <v>SalesContractNumber</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ref="F3:F66" si="4">ISNUMBER(SEARCH("~?",D3))</f>
@@ -10095,10 +10013,10 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G4" si="5">SUBSTITUTE(RIGHT(A3,B3-C3-1),";","")</f>
-        <v>string = null</v>
+        <v>string</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H66" si="6">IF(FIND("=",G3) &gt; -1, TRIM(LEFT(G3, FIND("=", G3) - 1)), G3)</f>
+        <f t="shared" ref="H3:H66" si="6">IF(ISNUMBER(SEARCH("=",G3)), TRIM(LEFT(G3, FIND("=", G3) - 1)), G3)</f>
         <v>string</v>
       </c>
       <c r="I3" t="b">
@@ -10123,28 +10041,28 @@
       </c>
       <c r="N3" s="2" t="str">
         <f t="shared" ref="N3:N4" si="11">"public "&amp;M3&amp;" "&amp;E3&amp;" { get; set; }"</f>
-        <v>public string Password { get; set; }</v>
+        <v>public string SalesContractNumber { get; set; }</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="2"/>
-        <v>Host</v>
+        <v>deliveryOrderNumber</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="3"/>
-        <v>Host</v>
+        <v>DeliveryOrderNumber</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" si="4"/>
@@ -10152,7 +10070,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="5"/>
-        <v>string = null</v>
+        <v>string</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="6"/>
@@ -10180,12 +10098,12 @@
       </c>
       <c r="N4" s="2" t="str">
         <f t="shared" si="11"/>
-        <v>public string Host { get; set; }</v>
+        <v>public string DeliveryOrderNumber { get; set; }</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B5">
         <f t="shared" ref="B5:B68" si="12">LEN(A5)</f>
@@ -10193,15 +10111,15 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C68" si="13">FIND(":", A5)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D68" si="14">LEFT(A5,C5-1)</f>
-        <v>Port</v>
+        <v>tradingPeriod</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="3"/>
-        <v>Port</v>
+        <v>TradingPeriod</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" si="4"/>
@@ -10209,11 +10127,11 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" ref="G5:G68" si="15">SUBSTITUTE(RIGHT(A5,B5-C5-1),";","")</f>
-        <v>number = null</v>
+        <v>Date</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="6"/>
-        <v>number</v>
+        <v>Date</v>
       </c>
       <c r="I5" t="b">
         <f t="shared" ref="I5:I68" si="16">ISNUMBER(SEARCH("[]",G5))</f>
@@ -10221,44 +10139,44 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="8"/>
-        <v>number</v>
+        <v>Date</v>
       </c>
       <c r="K5" t="str">
         <f>IFERROR(VLOOKUP(J5,Types!$F$3:$G$7,2,FALSE),J5)</f>
-        <v>int</v>
+        <v>DateTime</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="9"/>
-        <v>int</v>
+        <v>DateTime</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="10"/>
-        <v>int</v>
+        <v>DateTime</v>
       </c>
       <c r="N5" s="2" t="str">
         <f t="shared" ref="N5:N68" si="17">"public "&amp;M5&amp;" "&amp;E5&amp;" { get; set; }"</f>
-        <v>public int Port { get; set; }</v>
+        <v>public DateTime TradingPeriod { get; set; }</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B6">
         <f t="shared" si="12"/>
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <f t="shared" si="13"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="14"/>
-        <v>EnableSsl</v>
+        <v>currentPrice</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="3"/>
-        <v>EnableSsl</v>
+        <v>CurrentPrice</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" si="4"/>
@@ -10266,11 +10184,11 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="15"/>
-        <v>boolean = null</v>
+        <v>number</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="6"/>
-        <v>boolean</v>
+        <v>number</v>
       </c>
       <c r="I6" t="b">
         <f t="shared" si="16"/>
@@ -10278,44 +10196,44 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="8"/>
-        <v>boolean</v>
+        <v>number</v>
       </c>
       <c r="K6" t="str">
         <f>IFERROR(VLOOKUP(J6,Types!$F$3:$G$7,2,FALSE),J6)</f>
-        <v>bool</v>
+        <v>int</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="9"/>
-        <v>bool</v>
+        <v>int</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="10"/>
-        <v>bool</v>
+        <v>int</v>
       </c>
       <c r="N6" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>public bool EnableSsl { get; set; }</v>
+        <v>public int CurrentPrice { get; set; }</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B7">
         <f t="shared" si="12"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="14"/>
-        <v>From</v>
+        <v>proposedPrice</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="3"/>
-        <v>From</v>
+        <v>ProposedPrice</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" si="4"/>
@@ -10323,11 +10241,11 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="15"/>
-        <v>string = null</v>
+        <v>number</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="6"/>
-        <v>string</v>
+        <v>number</v>
       </c>
       <c r="I7" t="b">
         <f t="shared" si="16"/>
@@ -10335,44 +10253,44 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="8"/>
-        <v>string</v>
+        <v>number</v>
       </c>
       <c r="K7" t="str">
         <f>IFERROR(VLOOKUP(J7,Types!$F$3:$G$7,2,FALSE),J7)</f>
-        <v>string</v>
+        <v>int</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="9"/>
-        <v>string</v>
+        <v>int</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="10"/>
-        <v>string</v>
+        <v>int</v>
       </c>
       <c r="N7" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>public string From { get; set; }</v>
+        <v>public int ProposedPrice { get; set; }</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B8">
         <f t="shared" si="12"/>
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <f t="shared" si="13"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="14"/>
-        <v>FromDisplayName</v>
+        <v>createdBy</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="3"/>
-        <v>FromDisplayName</v>
+        <v>CreatedBy</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" si="4"/>
@@ -10380,7 +10298,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="15"/>
-        <v>string = null</v>
+        <v>string</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="6"/>
@@ -10408,28 +10326,28 @@
       </c>
       <c r="N8" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>public string FromDisplayName { get; set; }</v>
+        <v>public string CreatedBy { get; set; }</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B9">
         <f t="shared" si="12"/>
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <f t="shared" si="13"/>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="14"/>
-        <v>UseCredentials</v>
+        <v>created</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="3"/>
-        <v>UseCredentials</v>
+        <v>Created</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" si="4"/>
@@ -10437,11 +10355,11 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="15"/>
-        <v>boolean = null</v>
+        <v>Date</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="6"/>
-        <v>boolean</v>
+        <v>Date</v>
       </c>
       <c r="I9" t="b">
         <f t="shared" si="16"/>
@@ -10449,144 +10367,150 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="8"/>
-        <v>boolean</v>
+        <v>Date</v>
       </c>
       <c r="K9" t="str">
         <f>IFERROR(VLOOKUP(J9,Types!$F$3:$G$7,2,FALSE),J9)</f>
-        <v>bool</v>
+        <v>DateTime</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="9"/>
-        <v>bool</v>
+        <v>DateTime</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="10"/>
-        <v>bool</v>
+        <v>DateTime</v>
       </c>
       <c r="N9" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>public bool UseCredentials { get; set; }</v>
+        <v>public DateTime Created { get; set; }</v>
       </c>
     </row>
     <row r="10" spans="1:14">
+      <c r="A10" s="10" t="s">
+        <v>142</v>
+      </c>
       <c r="B10">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C10" t="e">
+        <v>17</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D10" t="e">
+        <v>9</v>
+      </c>
+      <c r="D10" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E10" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>currency</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v>Currency</v>
       </c>
       <c r="F10" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G10" t="e">
+      <c r="G10" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H10" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>string</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="6"/>
+        <v>string</v>
       </c>
       <c r="I10" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J10" t="e">
+      <c r="J10" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K10" t="e">
+        <v>string</v>
+      </c>
+      <c r="K10" t="str">
         <f>IFERROR(VLOOKUP(J10,Types!$F$3:$G$7,2,FALSE),J10)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L10" t="e">
+        <v>string</v>
+      </c>
+      <c r="L10" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M10" t="e">
+        <v>string</v>
+      </c>
+      <c r="M10" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N10" s="2" t="e">
+        <v>string</v>
+      </c>
+      <c r="N10" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>public string Currency { get; set; }</v>
       </c>
     </row>
     <row r="11" spans="1:14">
+      <c r="A11" s="10" t="s">
+        <v>136</v>
+      </c>
       <c r="B11">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C11" t="e">
+        <v>28</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D11" t="e">
+        <v>20</v>
+      </c>
+      <c r="D11" t="str">
         <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E11" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <v>deliveryOrderNumber</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v>DeliveryOrderNumber</v>
       </c>
       <c r="F11" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G11" t="e">
+      <c r="G11" t="str">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H11" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>string</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="6"/>
+        <v>string</v>
       </c>
       <c r="I11" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J11" t="e">
+      <c r="J11" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K11" t="e">
+        <v>string</v>
+      </c>
+      <c r="K11" t="str">
         <f>IFERROR(VLOOKUP(J11,Types!$F$3:$G$7,2,FALSE),J11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L11" t="e">
+        <v>string</v>
+      </c>
+      <c r="L11" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M11" t="e">
+        <v>string</v>
+      </c>
+      <c r="M11" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N11" s="2" t="e">
+        <v>string</v>
+      </c>
+      <c r="N11" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>public string DeliveryOrderNumber { get; set; }</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="B12">
-        <f t="shared" si="12"/>
+        <f>LEN(A12)</f>
         <v>0</v>
       </c>
       <c r="C12" t="e">
-        <f t="shared" si="13"/>
+        <f>FIND(":", A12)</f>
         <v>#VALUE!</v>
       </c>
       <c r="D12" t="e">
-        <f t="shared" si="14"/>
+        <f>LEFT(A12,C12-1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="E12" t="e">
@@ -10598,7 +10522,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="e">
-        <f t="shared" si="15"/>
+        <f>SUBSTITUTE(RIGHT(A12,B12-C12-1),";","")</f>
         <v>#VALUE!</v>
       </c>
       <c r="H12" t="e">
@@ -10631,438 +10555,462 @@
       </c>
     </row>
     <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>143</v>
+      </c>
       <c r="B13">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C13" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D13" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E13" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <f>LEN(A13)</f>
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <f>FIND(":", A13)</f>
+        <v>9</v>
+      </c>
+      <c r="D13" t="str">
+        <f>LEFT(A13,C13-1)</f>
+        <v>Username</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v>Username</v>
       </c>
       <c r="F13" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G13" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H13" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="G13" t="str">
+        <f>SUBSTITUTE(RIGHT(A13,B13-C13-1),";","")</f>
+        <v>string = null</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="6"/>
+        <v>string</v>
       </c>
       <c r="I13" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J13" t="e">
+      <c r="J13" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K13" t="e">
+        <v>string</v>
+      </c>
+      <c r="K13" t="str">
         <f>IFERROR(VLOOKUP(J13,Types!$F$3:$G$7,2,FALSE),J13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L13" t="e">
+        <v>string</v>
+      </c>
+      <c r="L13" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M13" t="e">
+        <v>string</v>
+      </c>
+      <c r="M13" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N13" s="2" t="e">
+        <v>string</v>
+      </c>
+      <c r="N13" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>public string Username { get; set; }</v>
       </c>
     </row>
     <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>144</v>
+      </c>
       <c r="B14">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C14" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D14" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E14" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <f>LEN(A14)</f>
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <f>FIND(":", A14)</f>
+        <v>9</v>
+      </c>
+      <c r="D14" t="str">
+        <f>LEFT(A14,C14-1)</f>
+        <v>Password</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v>Password</v>
       </c>
       <c r="F14" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G14" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H14" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="G14" t="str">
+        <f>SUBSTITUTE(RIGHT(A14,B14-C14-1),";","")</f>
+        <v>string = null</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="6"/>
+        <v>string</v>
       </c>
       <c r="I14" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J14" t="e">
+      <c r="J14" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K14" t="e">
+        <v>string</v>
+      </c>
+      <c r="K14" t="str">
         <f>IFERROR(VLOOKUP(J14,Types!$F$3:$G$7,2,FALSE),J14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L14" t="e">
+        <v>string</v>
+      </c>
+      <c r="L14" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M14" t="e">
+        <v>string</v>
+      </c>
+      <c r="M14" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N14" s="2" t="e">
+        <v>string</v>
+      </c>
+      <c r="N14" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>public string Password { get; set; }</v>
       </c>
     </row>
     <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>145</v>
+      </c>
       <c r="B15">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C15" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D15" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E15" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <f>LEN(A15)</f>
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <f>FIND(":", A15)</f>
+        <v>5</v>
+      </c>
+      <c r="D15" t="str">
+        <f>LEFT(A15,C15-1)</f>
+        <v>Host</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>Host</v>
       </c>
       <c r="F15" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G15" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H15" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="G15" t="str">
+        <f>SUBSTITUTE(RIGHT(A15,B15-C15-1),";","")</f>
+        <v>string = null</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="6"/>
+        <v>string</v>
       </c>
       <c r="I15" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J15" t="e">
+      <c r="J15" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K15" t="e">
+        <v>string</v>
+      </c>
+      <c r="K15" t="str">
         <f>IFERROR(VLOOKUP(J15,Types!$F$3:$G$7,2,FALSE),J15)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L15" t="e">
+        <v>string</v>
+      </c>
+      <c r="L15" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M15" t="e">
+        <v>string</v>
+      </c>
+      <c r="M15" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N15" s="2" t="e">
+        <v>string</v>
+      </c>
+      <c r="N15" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
+        <v>public string Host { get; set; }</v>
       </c>
     </row>
     <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>146</v>
+      </c>
       <c r="B16">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C16" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D16" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E16" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <f>LEN(A16)</f>
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <f>FIND(":", A16)</f>
+        <v>5</v>
+      </c>
+      <c r="D16" t="str">
+        <f>LEFT(A16,C16-1)</f>
+        <v>Port</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v>Port</v>
       </c>
       <c r="F16" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G16" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H16" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="G16" t="str">
+        <f>SUBSTITUTE(RIGHT(A16,B16-C16-1),";","")</f>
+        <v>number = null</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="6"/>
+        <v>number</v>
       </c>
       <c r="I16" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J16" t="e">
+      <c r="J16" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K16" t="e">
+        <v>number</v>
+      </c>
+      <c r="K16" t="str">
         <f>IFERROR(VLOOKUP(J16,Types!$F$3:$G$7,2,FALSE),J16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L16" t="e">
+        <v>int</v>
+      </c>
+      <c r="L16" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M16" t="e">
+        <v>int</v>
+      </c>
+      <c r="M16" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N16" s="2" t="e">
+        <v>int</v>
+      </c>
+      <c r="N16" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14">
+        <v>public int Port { get; set; }</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>147</v>
+      </c>
       <c r="B17">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C17" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D17" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E17" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <f>LEN(A17)</f>
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <f>FIND(":", A17)</f>
+        <v>10</v>
+      </c>
+      <c r="D17" t="str">
+        <f>LEFT(A17,C17-1)</f>
+        <v>EnableSsl</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v>EnableSsl</v>
       </c>
       <c r="F17" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G17" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H17" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="G17" t="str">
+        <f>SUBSTITUTE(RIGHT(A17,B17-C17-1),";","")</f>
+        <v>boolean = null</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="6"/>
+        <v>boolean</v>
       </c>
       <c r="I17" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J17" t="e">
+      <c r="J17" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K17" t="e">
+        <v>boolean</v>
+      </c>
+      <c r="K17" t="str">
         <f>IFERROR(VLOOKUP(J17,Types!$F$3:$G$7,2,FALSE),J17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L17" t="e">
+        <v>bool</v>
+      </c>
+      <c r="L17" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M17" t="e">
+        <v>bool</v>
+      </c>
+      <c r="M17" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N17" s="2" t="e">
+        <v>bool</v>
+      </c>
+      <c r="N17" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14">
+        <v>public bool EnableSsl { get; set; }</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>148</v>
+      </c>
       <c r="B18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C18" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D18" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E18" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <f>LEN(A18)</f>
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <f>FIND(":", A18)</f>
+        <v>5</v>
+      </c>
+      <c r="D18" t="str">
+        <f>LEFT(A18,C18-1)</f>
+        <v>From</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v>From</v>
       </c>
       <c r="F18" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G18" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H18" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="G18" t="str">
+        <f>SUBSTITUTE(RIGHT(A18,B18-C18-1),";","")</f>
+        <v>string = null</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="6"/>
+        <v>string</v>
       </c>
       <c r="I18" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J18" t="e">
+      <c r="J18" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K18" t="e">
+        <v>string</v>
+      </c>
+      <c r="K18" t="str">
         <f>IFERROR(VLOOKUP(J18,Types!$F$3:$G$7,2,FALSE),J18)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L18" t="e">
+        <v>string</v>
+      </c>
+      <c r="L18" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M18" t="e">
+        <v>string</v>
+      </c>
+      <c r="M18" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N18" s="2" t="e">
+        <v>string</v>
+      </c>
+      <c r="N18" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14">
+        <v>public string From { get; set; }</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
+        <v>149</v>
+      </c>
       <c r="B19">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C19" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D19" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <f>LEN(A19)</f>
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <f>FIND(":", A19)</f>
+        <v>16</v>
+      </c>
+      <c r="D19" t="str">
+        <f>LEFT(A19,C19-1)</f>
+        <v>FromDisplayName</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v>FromDisplayName</v>
       </c>
       <c r="F19" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G19" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H19" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="G19" t="str">
+        <f>SUBSTITUTE(RIGHT(A19,B19-C19-1),";","")</f>
+        <v>string = null</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="6"/>
+        <v>string</v>
       </c>
       <c r="I19" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J19" t="e">
+      <c r="J19" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K19" t="e">
+        <v>string</v>
+      </c>
+      <c r="K19" t="str">
         <f>IFERROR(VLOOKUP(J19,Types!$F$3:$G$7,2,FALSE),J19)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L19" t="e">
+        <v>string</v>
+      </c>
+      <c r="L19" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M19" t="e">
+        <v>string</v>
+      </c>
+      <c r="M19" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N19" s="2" t="e">
+        <v>string</v>
+      </c>
+      <c r="N19" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14">
+        <v>public string FromDisplayName { get; set; }</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
       <c r="B20">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="C20" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D20" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" t="e">
-        <f t="shared" si="3"/>
-        <v>#VALUE!</v>
+        <f>LEN(A20)</f>
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <f>FIND(":", A20)</f>
+        <v>15</v>
+      </c>
+      <c r="D20" t="str">
+        <f>LEFT(A20,C20-1)</f>
+        <v>UseCredentials</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v>UseCredentials</v>
       </c>
       <c r="F20" t="b">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G20" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H20" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+      <c r="G20" t="str">
+        <f>SUBSTITUTE(RIGHT(A20,B20-C20-1),";","")</f>
+        <v>boolean = null</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="6"/>
+        <v>boolean</v>
       </c>
       <c r="I20" t="b">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J20" t="e">
+      <c r="J20" t="str">
         <f t="shared" si="8"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K20" t="e">
+        <v>boolean</v>
+      </c>
+      <c r="K20" t="str">
         <f>IFERROR(VLOOKUP(J20,Types!$F$3:$G$7,2,FALSE),J20)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L20" t="e">
+        <v>bool</v>
+      </c>
+      <c r="L20" t="str">
         <f t="shared" si="9"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M20" t="e">
+        <v>bool</v>
+      </c>
+      <c r="M20" t="str">
         <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N20" s="2" t="e">
+        <v>bool</v>
+      </c>
+      <c r="N20" s="2" t="str">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14">
+        <v>public bool UseCredentials { get; set; }</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="B21">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11116,7 +11064,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="1:14">
       <c r="B22">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11170,7 +11118,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="1:14">
       <c r="B23">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11224,7 +11172,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="1:14">
       <c r="B24">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11278,7 +11226,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="1:14">
       <c r="B25">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11332,7 +11280,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="2:14">
+    <row r="26" spans="1:14">
       <c r="B26">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11386,7 +11334,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="2:14">
+    <row r="27" spans="1:14">
       <c r="B27">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11440,7 +11388,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="2:14">
+    <row r="28" spans="1:14">
       <c r="B28">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11494,7 +11442,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="1:14">
       <c r="B29">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11548,7 +11496,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="1:14">
       <c r="B30">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11602,7 +11550,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="1:14">
       <c r="B31">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -11656,7 +11604,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="1:14">
       <c r="B32">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -13572,7 +13520,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="H67" t="e">
-        <f t="shared" ref="H67:H90" si="20">IF(FIND("=",G67) &gt; -1, TRIM(LEFT(G67, FIND("=", G67) - 1)), G67)</f>
+        <f t="shared" ref="H67:H90" si="20">IF(ISNUMBER(SEARCH("=",G67)), TRIM(LEFT(G67, FIND("=", G67) - 1)), G67)</f>
         <v>#VALUE!</v>
       </c>
       <c r="I67" t="b">

</xml_diff>